<commit_message>
forgot to commit the xlsx
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="131">
   <si>
     <t>JSON</t>
   </si>
@@ -39,12 +39,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>&lt;OWNER&gt;&lt;/OWNER&gt;</t>
-  </si>
-  <si>
-    <t>&lt;SPECIES&gt;&lt;/SPECIES&gt;</t>
   </si>
   <si>
     <t>Owner of the pole</t>
@@ -69,9 +63,6 @@
 WC = Western Cedar</t>
   </si>
   <si>
-    <t xml:space="preserve">    &lt;AGL&gt;&lt;/AGL&gt;</t>
-  </si>
-  <si>
     <t>AGL</t>
   </si>
   <si>
@@ -88,9 +79,6 @@
     <t>AGL (ft-in)</t>
   </si>
   <si>
-    <t xml:space="preserve">    &lt;GLC&gt;&lt;/GLC&gt;</t>
-  </si>
-  <si>
     <t>GLC</t>
   </si>
   <si>
@@ -103,9 +91,6 @@
     <t>Ground level circumference. The circumference of the pole at the bottom.</t>
   </si>
   <si>
-    <t xml:space="preserve">    &lt;BASE&gt;&lt;/BASE&gt;</t>
-  </si>
-  <si>
     <t>Base</t>
   </si>
   <si>
@@ -119,12 +104,6 @@
   </si>
   <si>
     <t>[leads][locations][designs][structure][pole][clientItem][classOfPole]</t>
-  </si>
-  <si>
-    <t>[leads][locations][designs][structure][pole][clientItem][height]</t>
-  </si>
-  <si>
-    <t>Address</t>
   </si>
   <si>
     <t>[address][number]
@@ -138,9 +117,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t xml:space="preserve">    &lt;LOCDESC&gt;&lt;/LOCDESC&gt;</t>
-  </si>
-  <si>
     <t>Str. Location</t>
   </si>
   <si>
@@ -155,12 +131,6 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t xml:space="preserve">    &lt;GPS_LAT&gt;&lt;/GPS_LAT&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;GPS_LONG&gt;-&lt;/GPS_LONG&gt;</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -179,17 +149,306 @@
     <t>Pole Type</t>
   </si>
   <si>
-    <t>[leads][locations][forms][Pole Type]</t>
+    <t>The class of the pole is similar to the Quality. Low to High: 6,5,4,3,2,1,H1,H2,H3</t>
+  </si>
+  <si>
+    <t>The base is the type of material that the pole is set into. 
+E.g. Concrete, Dirt, etc.</t>
+  </si>
+  <si>
+    <t>Pole Ht.</t>
+  </si>
+  <si>
+    <t>The length of the entire pole including what is in the ground.</t>
+  </si>
+  <si>
+    <t>The pole type identifies whether the pole is carrying transmission, Distrobution, communication, or a combination of those.</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>See list of dictricts.</t>
+  </si>
+  <si>
+    <t>Date that the pole/project was completed.</t>
+  </si>
+  <si>
+    <t>Date Fielded</t>
+  </si>
+  <si>
+    <t>Field Date</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>[date]</t>
+  </si>
+  <si>
+    <t>Iff "Field Date" not found in JSON in then use Date</t>
+  </si>
+  <si>
+    <t>Project Address</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][pole][clientItem][height][value]</t>
+  </si>
+  <si>
+    <t>Structure Number</t>
+  </si>
+  <si>
+    <t>[leads][locations][label]</t>
+  </si>
+  <si>
+    <t>Pole No</t>
+  </si>
+  <si>
+    <t>Pole number for identification</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Whether the pole has comms or not</t>
+  </si>
+  <si>
+    <t>Wind Pounds</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][analysis]</t>
+  </si>
+  <si>
+    <t>There might be more than 1 analysis based on whether the pole is grandfathered.</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Year Installed</t>
+  </si>
+  <si>
+    <t>Yr In</t>
+  </si>
+  <si>
+    <t>[leads][locations][forms][fields][GrandFather]</t>
+  </si>
+  <si>
+    <t>Grandfather</t>
+  </si>
+  <si>
+    <t>Grandfather rule. If yes, will have 2 windloads</t>
+  </si>
+  <si>
+    <t>High Fire</t>
+  </si>
+  <si>
+    <t>High chance of their being fire</t>
+  </si>
+  <si>
+    <t>Height to Brand</t>
+  </si>
+  <si>
+    <t>[leads][locations][forms][0][fields][Pole Type]</t>
+  </si>
+  <si>
+    <t>[leads][locations][forms][0][fields][Field Inspection Date]</t>
+  </si>
+  <si>
+    <t>[leads][locations][forms][0][fields][High Fire]</t>
+  </si>
+  <si>
+    <t>[leads][locations][forms][0][fields][District]</t>
+  </si>
+  <si>
+    <t>[leads][locations][forms][1][fields][Year Installed]</t>
+  </si>
+  <si>
+    <t>[leads][locations][forms][1][fields][Brand Height]</t>
+  </si>
+  <si>
+    <t>Brand Height</t>
+  </si>
+  <si>
+    <t>Height to the brand (unsure if units)</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.WIRE&gt;&lt;POLE_ID&gt;&lt;/POLE_ID&gt;&lt;/CIP_SH.WIRE&gt;</t>
+  </si>
+  <si>
+    <t>Pole ID</t>
+  </si>
+  <si>
+    <t>Cyient created pole ID.</t>
+  </si>
+  <si>
+    <t>WEP ID</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][i][id]</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.WIRE&gt;&lt;WEP_ID&gt;&lt;/WEP_ID&gt;&lt;/CIP_SH.WIRE&gt;</t>
+  </si>
+  <si>
+    <t>Year the pole was put in the floor. Weirdly enough its not an int it’s a string in the JSON. If (FY_INST == NULL) then use YR_INST.</t>
+  </si>
+  <si>
+    <t>[i] can be any number because there can be multiple WEPS (wire end points). The number of individual WEP_ID is the number of WEPS in the XML</t>
+  </si>
+  <si>
+    <t>WEP #</t>
+  </si>
+  <si>
+    <t>Tension</t>
+  </si>
+  <si>
+    <t>See tension rules from previous emails</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.WIRE&gt;&lt;SLACK&gt;&lt;/SLACK&gt;&lt;/CIP_SH.WIRE&gt;</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][wires][tensionGroup]</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.WIRE&gt;&lt;USIZE&gt;&lt;/USIZE&gt;&lt;/CIP_SH.WIRE&gt;</t>
+  </si>
+  <si>
+    <t>Wire Size</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][wires][clientItem][size]</t>
+  </si>
+  <si>
+    <t>The size and type of wire</t>
+  </si>
+  <si>
+    <t>Wire Height</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.WIRE&gt;&lt;HEIGHT&gt;&lt;/HEIGHT&gt;&lt;/CIP_SH.WIRE&gt;</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][wires][attachmentHeight][value]</t>
+  </si>
+  <si>
+    <t>The height where the wire is attached to the pole.</t>
+  </si>
+  <si>
+    <t>Usage Group</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][wires][usageGroup]</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.WIRE&gt;&lt;WIRE_TYPE&gt;&lt;/WIRE_TYPE&gt;&lt;/CIP_SH.WIRE&gt;</t>
+  </si>
+  <si>
+    <t>Wire Selection</t>
+  </si>
+  <si>
+    <t>Attache Height</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][owner][industry]</t>
+  </si>
+  <si>
+    <t>See rules from email</t>
+  </si>
+  <si>
+    <t>XMLOwner</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.WIRE&gt;&lt;OWNER&gt;&lt;/OWNER&gt;&lt;/CIP_SH.WIRE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;OWNER&gt;&lt;/OWNER&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;SPECIES&gt;&lt;/SPECIES&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;Pole&gt;&lt;AGL&gt;&lt;/AGL&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;GLC&gt;&lt;/GLC&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;BASE&gt;&lt;/BASE&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;FCLASS&gt;&lt;/FCLASS&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;FHEIGHT&gt;&lt;/FHEIGHT&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;LOCDESC&gt;&lt;/LOCDESC&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;GPS_LAT&gt;&lt;/GPS_LAT&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;GPS_LONG&gt;-&lt;/GPS_LONG&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;UUSAGE&gt;&lt;/UUSAGE&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;DISTRICT&gt;&lt;/DISTRICT&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;FCCOMPDATE&gt;&lt;/FCCOMPDATE&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;FSTRUCNUM&gt;&lt;/FSTRUCNUM&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;GRADE&gt;&lt;/GRADE&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;WIND_POUND_RATING&gt;&lt;/WIND_POUND_RATING&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;FYR_INST&gt;&lt;/FYR_INST&gt;
+&lt;YR_INST&gt;&lt;/YR_INST&gt;
+&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;GRAND_FATHER&gt;&lt;/GRAND_FATHER&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;HF&gt;&lt;/HF&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pole&gt;&lt;HGTOFBRAND&gt;&lt;/HGTOFBRAND&gt;&lt;/Pole&gt;</t>
+  </si>
+  <si>
+    <t>xml owner is different from pdf owner please keep as a different variable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,16 +474,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -235,6 +501,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E32" totalsRowShown="0">
+  <autoFilter ref="A1:E32"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Key"/>
+    <tableColumn id="2" name="JSON"/>
+    <tableColumn id="3" name="XML"/>
+    <tableColumn id="4" name="PDF"/>
+    <tableColumn id="5" name="Description" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -500,17 +780,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="51.5703125" customWidth="1"/>
@@ -535,176 +815,524 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
xlsx wont commit properly
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -448,7 +448,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -782,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added the new PDF that is needed in between other pages. Added the equipment, insulator, and crossarm info to the schema xlsx
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="186">
   <si>
     <t>JSON</t>
   </si>
@@ -106,22 +106,10 @@
     <t>[leads][locations][designs][structure][pole][clientItem][classOfPole]</t>
   </si>
   <si>
-    <t>[address][number]
-[address][street]
-[address][city]
-[address][country]
-[address][state]
-[address][zip_code]</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
     <t>Str. Location</t>
-  </si>
-  <si>
-    <t>Formal mailing address
-e.g. 9050 Archibald ave, Rancho Cucamonga, Ca, 91730</t>
   </si>
   <si>
     <t>Location relative to nearest street.
@@ -187,9 +175,6 @@
   </si>
   <si>
     <t>Iff "Field Date" not found in JSON in then use Date</t>
-  </si>
-  <si>
-    <t>Project Address</t>
   </si>
   <si>
     <t>[leads][locations][designs][structure][pole][clientItem][height][value]</t>
@@ -432,6 +417,180 @@
   </si>
   <si>
     <t>xml owner is different from pdf owner please keep as a different variable</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][insulators][clientItem]</t>
+  </si>
+  <si>
+    <t>Insulator Size</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.INSULATOR&gt;&lt;USIZE&gt;&lt;/USIZE&gt;&lt;/CIP_SH.INSULATOR&gt;</t>
+  </si>
+  <si>
+    <t>The size of the insulator selected.</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][equipments][clientItem][size]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;CIP_SH.EQUIPMENT&gt;&lt;USIZE&gt;&lt;/USIZE&gt; &lt;/CIP_SH.EQUIPMENT&gt;</t>
+  </si>
+  <si>
+    <t>Equipment Size</t>
+  </si>
+  <si>
+    <t>kV - Insulator Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See the rules from previous emails for equipment. (There should be an "E" [for equipment] in the WEP # and the size should go in wire selection} </t>
+  </si>
+  <si>
+    <t>Crossarm Size</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][crossArms][clientItem]</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.CROSSARM&gt;&lt;USIZE&gt;&lt;/USIZE&gt;&lt;CIP_SH.CROSSARM&gt;</t>
+  </si>
+  <si>
+    <t>Cross Arm Size</t>
+  </si>
+  <si>
+    <t>The size of the cross arm</t>
+  </si>
+  <si>
+    <t>Insulator Height</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][insulators][attachmentHeight][value]</t>
+  </si>
+  <si>
+    <t>Insulator Offset</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][insulators][offset][value]</t>
+  </si>
+  <si>
+    <t>Insulator Direction</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][insulators][direction]</t>
+  </si>
+  <si>
+    <t>Insulator Double</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][insulators][doubleInsulator]</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.INSULATOR&gt;&lt;HEIGHT&gt;&lt;/HEIGHT&gt;&lt;/CIP_SH.INSULATOR&gt;</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.INSULATOR&gt;&lt;OFFSET&gt;&lt;/OFFSET&gt;&lt;/CIP_SH.INSULATOR&gt;</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.INSULATOR&gt;&lt;ANGLE&gt;&lt;/ANGLE&gt;&lt;/CIP_SH.INSULATOR&gt;</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.INSULATOR&gt;&lt;DBLINSULATED&gt;&lt;/DBLINSULATED&gt;&lt;/CIP_SH.INSULATOR&gt;</t>
+  </si>
+  <si>
+    <t>Equipment Type</t>
+  </si>
+  <si>
+    <t>Equipment Height</t>
+  </si>
+  <si>
+    <t>Equipment Owner</t>
+  </si>
+  <si>
+    <t>Equipment Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;CIP_SH.EQUIPMENT&gt;&lt;EQUIPTYPE&gt;&lt;/EQUIPTYPE&gt;&lt;/CIP_SH.EQUIPMENT&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;CIP_SH.EQUIPMENT&gt;&lt;HEIGHT&gt;&lt;/HEIGHT&gt;&lt;/CIP_SH.EQUIPMENT&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;CIP_SH.EQUIPMENT&gt;&lt;ANGLE&gt;&lt;/ANGLE&gt;&lt;/CIP_SH.EQUIPMENT&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;CIP_SH.EQUIPMENT&gt;&lt;OWNER&gt;&lt;/OWNER&gt;&lt;/CIP_SH.EQUIPMENT&gt;</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][equipments][clientItem][type]</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][equipments][attachmentHeight][value]</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][equipments][direction]</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][equipments][owner][id]</t>
+  </si>
+  <si>
+    <t>Crossarm Height</t>
+  </si>
+  <si>
+    <t>Crossarm Direction</t>
+  </si>
+  <si>
+    <t>Crossarm Offset</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][crossArms][attachmentHeight][value]</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][crossArms][direction]</t>
+  </si>
+  <si>
+    <t>[leads][locations][designs][structure][wireEndPoints][crossArms][offset][value]</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.CROSSARM&gt;&lt;HEIGHT&gt;&lt;/HEIGHT&gt;&lt;CIP_SH.CROSSARM&gt;</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.CROSSARM&gt;&lt;ANGLE&gt;&lt;/ANGLE&gt;&lt;CIP_SH.CROSSARM&gt;</t>
+  </si>
+  <si>
+    <t>&lt;CIP_SH.CROSSARM&gt;&lt;OFFSET&gt;&lt;/OFFSET&gt;&lt;CIP_SH.CROSSARM&gt;</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Attach Height</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>The category the equipment is in.</t>
+  </si>
+  <si>
+    <t>The height where the equipment is attached to the pole.</t>
+  </si>
+  <si>
+    <t>The Azimuth of the Equipment</t>
+  </si>
+  <si>
+    <t>The owner of the equipment</t>
+  </si>
+  <si>
+    <t>The height where the crossarm is attached to the pole.</t>
+  </si>
+  <si>
+    <t>The Azimuth of the Crossarm</t>
+  </si>
+  <si>
+    <t>How far alonmg the x axis the crossarm is attached to the pole</t>
   </si>
 </sst>
 </file>
@@ -503,8 +662,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E32" totalsRowShown="0">
-  <autoFilter ref="A1:E32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E45" totalsRowShown="0">
+  <autoFilter ref="A1:E45"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Key"/>
     <tableColumn id="2" name="JSON"/>
@@ -779,18 +938,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="81.140625" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="51.5703125" customWidth="1"/>
   </cols>
@@ -820,7 +979,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -837,7 +996,7 @@
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -854,7 +1013,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -871,7 +1030,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -885,13 +1044,13 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -902,13 +1061,13 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -916,302 +1075,302 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
         <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
-        <v>71</v>
-      </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>56</v>
       </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" t="s">
-        <v>125</v>
+        <v>71</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>126</v>
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>124</v>
       </c>
       <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
         <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" t="s">
-        <v>129</v>
-      </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
         <v>79</v>
       </c>
-      <c r="B24" t="s">
-        <v>9</v>
-      </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>85</v>
@@ -1219,112 +1378,309 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
         <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>92</v>
       </c>
       <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
         <v>93</v>
       </c>
-      <c r="C27" t="s">
-        <v>91</v>
-      </c>
       <c r="D27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>105</v>
+        <v>6</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" t="s">
         <v>100</v>
       </c>
-      <c r="B31" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>130</v>
+      <c r="E37" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>154</v>
+      </c>
+      <c r="B38" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38" t="s">
+        <v>158</v>
+      </c>
+      <c r="D38" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B39" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" t="s">
+        <v>159</v>
+      </c>
+      <c r="D39" t="s">
+        <v>176</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>157</v>
+      </c>
+      <c r="B40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" t="s">
+        <v>160</v>
+      </c>
+      <c r="D40" t="s">
+        <v>177</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" t="s">
+        <v>161</v>
+      </c>
+      <c r="D41" t="s">
+        <v>178</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" t="s">
+        <v>140</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43" t="s">
+        <v>169</v>
+      </c>
+      <c r="C43" t="s">
+        <v>172</v>
+      </c>
+      <c r="D43" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>167</v>
+      </c>
+      <c r="B44" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" t="s">
+        <v>177</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>168</v>
+      </c>
+      <c r="B45" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" t="s">
+        <v>174</v>
+      </c>
+      <c r="D45" t="s">
+        <v>178</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>